<commit_message>
refactor: add a makefile for better handling of high-level functions
</commit_message>
<xml_diff>
--- a/data/expected_stats.xlsx
+++ b/data/expected_stats.xlsx
@@ -423,10 +423,10 @@
         <v>17.52923840917323</v>
       </c>
       <c r="E2">
-        <v>0.04872269871584915</v>
+        <v>0.04887186309074776</v>
       </c>
       <c r="F2">
-        <v>17.56199708184831</v>
+        <v>17.52923840917323</v>
       </c>
       <c r="G2">
         <v>0.04567022432261091</v>

</xml_diff>

<commit_message>
feat: add a couple of local files
</commit_message>
<xml_diff>
--- a/data/expected_stats.xlsx
+++ b/data/expected_stats.xlsx
@@ -360,85 +360,85 @@
     <row r="1" s="1" customFormat="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>fishers_z_est</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>fishers_z_t_value</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>hsma_est</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>hsma_t_value</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>re_est</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>re_t_value</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>uwls_est</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>uwls_t_value</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>uwls3_est</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>uwls3_t_value</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>hsma_est</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>hsma_t_value</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>fishers_z_est</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>fishers_z_t_value</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2">
+        <v>0.06030813277927358</v>
+      </c>
+      <c r="B2">
+        <v>16.24184553868096</v>
+      </c>
+      <c r="C2">
+        <v>0.04567022432261091</v>
+      </c>
+      <c r="D2">
+        <v>17.6906469956982</v>
+      </c>
+      <c r="E2">
         <v>0.05914186723756871</v>
       </c>
-      <c r="B2">
+      <c r="F2">
         <v>16.42125501540017</v>
       </c>
-      <c r="C2">
+      <c r="G2">
         <v>0.04887186309074776</v>
       </c>
-      <c r="D2">
+      <c r="H2">
         <v>17.52923840917323</v>
       </c>
-      <c r="E2">
-        <v>0.04887186309074776</v>
-      </c>
-      <c r="F2">
-        <v>17.52923840917323</v>
-      </c>
-      <c r="G2">
-        <v>0.04567022432261091</v>
-      </c>
-      <c r="H2">
-        <v>17.6906469956982</v>
-      </c>
       <c r="I2">
-        <v>0.06030813277927358</v>
+        <v>0.04872269871584915</v>
       </c>
       <c r="J2">
-        <v>16.24184553868096</v>
+        <v>17.56199708184831</v>
       </c>
     </row>
   </sheetData>

</xml_diff>